<commit_message>
enhance page add selenium driver code
</commit_message>
<xml_diff>
--- a/Data Files/xls/data.xlsx
+++ b/Data Files/xls/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Katalon Studio\test\Data Files\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D761C3B2-C1BB-49C3-A8E7-3608E3E11EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66A9541-69C6-4B44-BA75-DA246696706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{3983194C-EAD8-4973-ABB9-EC535812B7F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3983194C-EAD8-4973-ABB9-EC535812B7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B498FC3-4B92-4BA8-83BF-1015E0D2A64A}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -522,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997A57E7-26DA-4FC8-8D87-1CBE7F521767}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>